<commit_message>
Updated SENDIG references to SDTM 1.2 and 1.3 data elements.
</commit_message>
<xml_diff>
--- a/import-files/sendig-3-0.xlsx
+++ b/import-files/sendig-3-0.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7493" uniqueCount="2589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7490" uniqueCount="2583">
   <si>
     <t>mms:context</t>
   </si>
@@ -7686,9 +7686,6 @@
     <t>sdtm-1-2:DataElement.Intervention.--LOC</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Intervention.--METHOD</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Intervention.--TRTV</t>
   </si>
   <si>
@@ -7701,18 +7698,6 @@
     <t>sdtm-1-2:DataElement.Intervention.--ADJ</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Intervention.--DUR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Intervention.--ELTM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Intervention.--TPTREF</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Intervention.--RFTDTC</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Event.--TERM</t>
   </si>
   <si>
@@ -7752,21 +7737,6 @@
     <t>sdtm-1-2:DataElement.Finding.--FAST</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--EXCLFL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--REASEX</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--ELTM</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--TPTREF</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--RFTDTC</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Identifier.--GRPID</t>
   </si>
   <si>
@@ -7806,21 +7776,12 @@
     <t>sdtm-1-2:DataElement.Finding.--NAM</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--LEAD</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Finding.--METHOD</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--CSTATE</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Finding.--DRVFL</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--EVLINT</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Finding.--ORNRLO</t>
   </si>
   <si>
@@ -7842,24 +7803,9 @@
     <t>sdtm-1-2:DataElement.Finding.--SPEC</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--ANTREG</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Finding.--SPCCND</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--SPCUFL</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--LAT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--DIR</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--PORTOT</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Finding.--TOX</t>
   </si>
   <si>
@@ -7872,15 +7818,6 @@
     <t>sdtm-1-2:DataElement.Finding.--LLOQ</t>
   </si>
   <si>
-    <t>sdtm-1-2:DataElement.Finding.--STINT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--ENINT</t>
-  </si>
-  <si>
-    <t>sdtm-1-2:DataElement.Finding.--DETECT</t>
-  </si>
-  <si>
     <t>sdtm-1-2:DataElement.Timing.EPOCH</t>
   </si>
   <si>
@@ -7909,6 +7846,51 @@
   </si>
   <si>
     <t>sdtm-1-2:DataElement.Timing.VISITDY</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--ANTREG</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--EXCLFL</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--REASEX</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--LEAD</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--CSTATE</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--SPCUFL</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--LAT</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--DIR</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Finding.--PORTOT</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--DUR</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--ELTM</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--TPTREF</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--RFTDTC</t>
+  </si>
+  <si>
+    <t>sdtm-1-2:DataElement.Timing.--EVLINT</t>
+  </si>
+  <si>
+    <t>sdtm-1-3:DataElement.Timing.--DETECT</t>
   </si>
 </sst>
 </file>
@@ -10104,7 +10086,7 @@
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -10804,7 +10786,7 @@
     <col min="1" max="1" width="39.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="98.85546875" style="9" customWidth="1"/>
@@ -11009,7 +10991,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>2580</v>
+        <v>2559</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>151</v>
@@ -11047,7 +11029,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>153</v>
@@ -11834,7 +11816,7 @@
         <v>11</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>146</v>
@@ -11872,7 +11854,7 @@
         <v>12</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>574</v>
@@ -12114,7 +12096,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>2580</v>
+        <v>2559</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>404</v>
@@ -12152,7 +12134,7 @@
         <v>8</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>407</v>
@@ -12735,9 +12717,6 @@
       <c r="C55" s="13">
         <v>15</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>2514</v>
-      </c>
       <c r="E55" s="9" t="s">
         <v>593</v>
       </c>
@@ -12771,7 +12750,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>2515</v>
+        <v>2514</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>237</v>
@@ -12806,7 +12785,7 @@
         <v>17</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>238</v>
@@ -12841,7 +12820,7 @@
         <v>18</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>239</v>
@@ -12882,7 +12861,7 @@
         <v>19</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>240</v>
@@ -12917,7 +12896,7 @@
         <v>20</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>2580</v>
+        <v>2559</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>242</v>
@@ -12955,7 +12934,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>244</v>
@@ -12993,7 +12972,7 @@
         <v>22</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>2584</v>
+        <v>2563</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>246</v>
@@ -13028,7 +13007,7 @@
         <v>23</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>248</v>
@@ -13063,7 +13042,7 @@
         <v>24</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>2519</v>
+        <v>2577</v>
       </c>
       <c r="E64" s="9" t="s">
         <v>250</v>
@@ -13101,7 +13080,7 @@
         <v>25</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>2586</v>
+        <v>2565</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>252</v>
@@ -13136,7 +13115,7 @@
         <v>26</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>2587</v>
+        <v>2566</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>253</v>
@@ -13171,7 +13150,7 @@
         <v>27</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>2520</v>
+        <v>2578</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>255</v>
@@ -13209,7 +13188,7 @@
         <v>28</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>2521</v>
+        <v>2579</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>256</v>
@@ -13244,7 +13223,7 @@
         <v>29</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>2522</v>
+        <v>2580</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>609</v>
@@ -13425,7 +13404,7 @@
         <v>5</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>2523</v>
+        <v>2518</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>174</v>
@@ -13460,7 +13439,7 @@
         <v>6</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>2524</v>
+        <v>2519</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>176</v>
@@ -13501,7 +13480,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>44</v>
@@ -13536,7 +13515,7 @@
         <v>8</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>2580</v>
+        <v>2559</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>178</v>
@@ -13574,7 +13553,7 @@
         <v>9</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>2584</v>
+        <v>2563</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>179</v>
@@ -13752,7 +13731,7 @@
         <v>5</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E83" s="9" t="s">
         <v>621</v>
@@ -13793,7 +13772,7 @@
         <v>6</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E84" s="9" t="s">
         <v>625</v>
@@ -13834,7 +13813,7 @@
         <v>7</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E85" s="9" t="s">
         <v>629</v>
@@ -13869,7 +13848,7 @@
         <v>8</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E86" s="9" t="s">
         <v>631</v>
@@ -13910,7 +13889,7 @@
         <v>9</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>634</v>
@@ -13945,7 +13924,7 @@
         <v>10</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>637</v>
@@ -13980,7 +13959,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E89" s="9" t="s">
         <v>640</v>
@@ -14021,7 +14000,7 @@
         <v>12</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E90" s="9" t="s">
         <v>643</v>
@@ -14062,7 +14041,7 @@
         <v>13</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E91" s="9" t="s">
         <v>646</v>
@@ -14097,7 +14076,7 @@
         <v>14</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>2534</v>
+        <v>2529</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>648</v>
@@ -14138,7 +14117,7 @@
         <v>15</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>2535</v>
+        <v>2530</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>650</v>
@@ -14179,7 +14158,7 @@
         <v>16</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>652</v>
@@ -14220,7 +14199,7 @@
         <v>17</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>655</v>
@@ -14255,7 +14234,7 @@
         <v>18</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>44</v>
@@ -14290,7 +14269,7 @@
         <v>19</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>660</v>
@@ -14328,7 +14307,7 @@
         <v>20</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>663</v>
@@ -14506,7 +14485,7 @@
         <v>5</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E103" s="9" t="s">
         <v>667</v>
@@ -14547,7 +14526,7 @@
         <v>6</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E104" s="9" t="s">
         <v>670</v>
@@ -14588,7 +14567,7 @@
         <v>7</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E105" s="9" t="s">
         <v>673</v>
@@ -14623,7 +14602,7 @@
         <v>8</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>675</v>
@@ -14664,7 +14643,7 @@
         <v>9</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E107" s="9" t="s">
         <v>676</v>
@@ -14699,7 +14678,7 @@
         <v>10</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E108" s="9" t="s">
         <v>678</v>
@@ -14734,7 +14713,7 @@
         <v>11</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E109" s="9" t="s">
         <v>680</v>
@@ -14775,7 +14754,7 @@
         <v>12</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E110" s="9" t="s">
         <v>682</v>
@@ -14816,7 +14795,7 @@
         <v>13</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E111" s="9" t="s">
         <v>685</v>
@@ -14851,7 +14830,7 @@
         <v>14</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E112" s="9" t="s">
         <v>687</v>
@@ -14892,7 +14871,7 @@
         <v>15</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E113" s="9" t="s">
         <v>688</v>
@@ -14927,7 +14906,7 @@
         <v>16</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E114" s="9" t="s">
         <v>690</v>
@@ -14965,7 +14944,7 @@
         <v>17</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E115" s="9" t="s">
         <v>692</v>
@@ -15003,7 +14982,7 @@
         <v>18</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E116" s="9" t="s">
         <v>695</v>
@@ -15038,7 +15017,7 @@
         <v>19</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E117" s="9" t="s">
         <v>697</v>
@@ -15073,7 +15052,7 @@
         <v>20</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>2538</v>
+        <v>2578</v>
       </c>
       <c r="E118" s="9" t="s">
         <v>700</v>
@@ -15111,7 +15090,7 @@
         <v>21</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E119" s="9" t="s">
         <v>702</v>
@@ -15146,7 +15125,7 @@
         <v>22</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E120" s="9" t="s">
         <v>704</v>
@@ -15359,7 +15338,7 @@
         <v>6</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E126" s="9" t="s">
         <v>708</v>
@@ -15394,7 +15373,7 @@
         <v>7</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E127" s="9" t="s">
         <v>711</v>
@@ -15429,7 +15408,7 @@
         <v>8</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E128" s="9" t="s">
         <v>714</v>
@@ -15464,7 +15443,7 @@
         <v>9</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E129" s="9" t="s">
         <v>716</v>
@@ -15499,7 +15478,7 @@
         <v>10</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="E130" s="9" t="s">
         <v>718</v>
@@ -15540,7 +15519,7 @@
         <v>11</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="E131" s="9" t="s">
         <v>722</v>
@@ -15575,7 +15554,7 @@
         <v>12</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>2545</v>
+        <v>2535</v>
       </c>
       <c r="E132" s="9" t="s">
         <v>725</v>
@@ -15616,7 +15595,7 @@
         <v>13</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E133" s="9" t="s">
         <v>728</v>
@@ -15651,7 +15630,7 @@
         <v>14</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E134" s="9" t="s">
         <v>730</v>
@@ -15686,7 +15665,7 @@
         <v>15</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>2546</v>
+        <v>2536</v>
       </c>
       <c r="E135" s="9" t="s">
         <v>732</v>
@@ -15721,7 +15700,7 @@
         <v>16</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E136" s="9" t="s">
         <v>734</v>
@@ -15762,7 +15741,7 @@
         <v>17</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E137" s="9" t="s">
         <v>736</v>
@@ -15797,7 +15776,7 @@
         <v>18</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>2547</v>
+        <v>2537</v>
       </c>
       <c r="E138" s="9" t="s">
         <v>738</v>
@@ -15832,7 +15811,7 @@
         <v>19</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E139" s="9" t="s">
         <v>741</v>
@@ -15867,7 +15846,7 @@
         <v>20</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>2549</v>
+        <v>2539</v>
       </c>
       <c r="E140" s="9" t="s">
         <v>743</v>
@@ -15902,7 +15881,7 @@
         <v>21</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E141" s="9" t="s">
         <v>745</v>
@@ -15943,7 +15922,7 @@
         <v>22</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E142" s="9" t="s">
         <v>746</v>
@@ -15978,7 +15957,7 @@
         <v>23</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>44</v>
@@ -16013,7 +15992,7 @@
         <v>24</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>748</v>
@@ -16051,7 +16030,7 @@
         <v>25</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>750</v>
@@ -16086,7 +16065,7 @@
         <v>26</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>2586</v>
+        <v>2565</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>753</v>
@@ -16121,7 +16100,7 @@
         <v>27</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>2587</v>
+        <v>2566</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>755</v>
@@ -16156,7 +16135,7 @@
         <v>28</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>2538</v>
+        <v>2578</v>
       </c>
       <c r="E148" s="9" t="s">
         <v>756</v>
@@ -16194,7 +16173,7 @@
         <v>29</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>758</v>
@@ -16229,7 +16208,7 @@
         <v>30</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E150" s="9" t="s">
         <v>760</v>
@@ -16410,7 +16389,7 @@
         <v>5</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E155" s="9" t="s">
         <v>763</v>
@@ -16451,7 +16430,7 @@
         <v>6</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E156" s="9" t="s">
         <v>767</v>
@@ -16492,7 +16471,7 @@
         <v>7</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E157" s="9" t="s">
         <v>771</v>
@@ -16527,7 +16506,7 @@
         <v>8</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E158" s="9" t="s">
         <v>773</v>
@@ -16562,7 +16541,7 @@
         <v>9</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>2546</v>
+        <v>2536</v>
       </c>
       <c r="E159" s="9" t="s">
         <v>775</v>
@@ -16597,7 +16576,7 @@
         <v>10</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E160" s="9" t="s">
         <v>777</v>
@@ -16632,7 +16611,7 @@
         <v>11</v>
       </c>
       <c r="D161" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E161" s="9" t="s">
         <v>779</v>
@@ -16670,7 +16649,7 @@
         <v>12</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E162" s="9" t="s">
         <v>782</v>
@@ -16848,7 +16827,7 @@
         <v>5</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E167" s="9" t="s">
         <v>181</v>
@@ -16883,7 +16862,7 @@
         <v>6</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="E168" s="9" t="s">
         <v>182</v>
@@ -16918,7 +16897,7 @@
         <v>7</v>
       </c>
       <c r="D169" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E169" s="9" t="s">
         <v>183</v>
@@ -16953,7 +16932,7 @@
         <v>8</v>
       </c>
       <c r="D170" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E170" s="9" t="s">
         <v>184</v>
@@ -16994,7 +16973,7 @@
         <v>9</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E171" s="9" t="s">
         <v>187</v>
@@ -17035,7 +17014,7 @@
         <v>10</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="E172" s="9" t="s">
         <v>190</v>
@@ -17076,7 +17055,7 @@
         <v>11</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>2551</v>
+        <v>2541</v>
       </c>
       <c r="E173" s="9" t="s">
         <v>192</v>
@@ -17117,7 +17096,7 @@
         <v>12</v>
       </c>
       <c r="D174" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E174" s="9" t="s">
         <v>195</v>
@@ -17152,7 +17131,7 @@
         <v>13</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E175" s="9" t="s">
         <v>196</v>
@@ -17193,7 +17172,7 @@
         <v>14</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E176" s="9" t="s">
         <v>197</v>
@@ -17234,7 +17213,7 @@
         <v>15</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E177" s="9" t="s">
         <v>199</v>
@@ -17269,7 +17248,7 @@
         <v>16</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E178" s="9" t="s">
         <v>201</v>
@@ -17310,7 +17289,7 @@
         <v>17</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E179" s="9" t="s">
         <v>202</v>
@@ -17351,7 +17330,7 @@
         <v>18</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E180" s="9" t="s">
         <v>203</v>
@@ -17386,7 +17365,7 @@
         <v>19</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>2552</v>
+        <v>2542</v>
       </c>
       <c r="E181" s="9" t="s">
         <v>204</v>
@@ -17421,7 +17400,7 @@
         <v>20</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>2553</v>
+        <v>2543</v>
       </c>
       <c r="E182" s="9" t="s">
         <v>206</v>
@@ -17456,7 +17435,7 @@
         <v>21</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>2554</v>
+        <v>2571</v>
       </c>
       <c r="E183" s="9" t="s">
         <v>796</v>
@@ -17497,7 +17476,7 @@
         <v>22</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>2555</v>
+        <v>2544</v>
       </c>
       <c r="E184" s="9" t="s">
         <v>209</v>
@@ -17538,7 +17517,7 @@
         <v>23</v>
       </c>
       <c r="D185" s="9" t="s">
-        <v>2556</v>
+        <v>2572</v>
       </c>
       <c r="E185" s="9" t="s">
         <v>801</v>
@@ -17579,7 +17558,7 @@
         <v>24</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>2534</v>
+        <v>2529</v>
       </c>
       <c r="E186" s="9" t="s">
         <v>212</v>
@@ -17620,7 +17599,7 @@
         <v>25</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>2557</v>
+        <v>2545</v>
       </c>
       <c r="E187" s="9" t="s">
         <v>213</v>
@@ -17661,7 +17640,7 @@
         <v>26</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E188" s="9" t="s">
         <v>214</v>
@@ -17696,7 +17675,7 @@
         <v>27</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E189" s="9" t="s">
         <v>806</v>
@@ -17737,7 +17716,7 @@
         <v>28</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E190" s="9" t="s">
         <v>807</v>
@@ -17772,7 +17751,7 @@
         <v>29</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E191" s="9" t="s">
         <v>44</v>
@@ -17807,7 +17786,7 @@
         <v>30</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E192" s="9" t="s">
         <v>215</v>
@@ -17845,7 +17824,7 @@
         <v>31</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E193" s="9" t="s">
         <v>810</v>
@@ -17883,7 +17862,7 @@
         <v>32</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E194" s="9" t="s">
         <v>217</v>
@@ -17918,7 +17897,7 @@
         <v>33</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E195" s="9" t="s">
         <v>815</v>
@@ -17953,7 +17932,7 @@
         <v>34</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>2586</v>
+        <v>2565</v>
       </c>
       <c r="E196" s="9" t="s">
         <v>218</v>
@@ -17988,7 +17967,7 @@
         <v>35</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>2587</v>
+        <v>2566</v>
       </c>
       <c r="E197" s="9" t="s">
         <v>219</v>
@@ -18023,7 +18002,7 @@
         <v>36</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>2538</v>
+        <v>2578</v>
       </c>
       <c r="E198" s="9" t="s">
         <v>221</v>
@@ -18061,7 +18040,7 @@
         <v>37</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E199" s="9" t="s">
         <v>222</v>
@@ -18096,7 +18075,7 @@
         <v>38</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E200" s="9" t="s">
         <v>223</v>
@@ -18134,7 +18113,7 @@
         <v>39</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>2558</v>
+        <v>2581</v>
       </c>
       <c r="E201" s="9" t="s">
         <v>821</v>
@@ -18347,7 +18326,7 @@
         <v>6</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E207" s="9" t="s">
         <v>826</v>
@@ -18382,7 +18361,7 @@
         <v>7</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E208" s="9" t="s">
         <v>827</v>
@@ -18423,7 +18402,7 @@
         <v>8</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E209" s="9" t="s">
         <v>831</v>
@@ -18464,7 +18443,7 @@
         <v>9</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E210" s="9" t="s">
         <v>835</v>
@@ -18499,7 +18478,7 @@
         <v>10</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E211" s="9" t="s">
         <v>836</v>
@@ -18540,7 +18519,7 @@
         <v>11</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E212" s="9" t="s">
         <v>837</v>
@@ -18575,7 +18554,7 @@
         <v>12</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E213" s="9" t="s">
         <v>839</v>
@@ -18610,7 +18589,7 @@
         <v>13</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E214" s="9" t="s">
         <v>841</v>
@@ -18651,7 +18630,7 @@
         <v>14</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E215" s="9" t="s">
         <v>843</v>
@@ -18692,7 +18671,7 @@
         <v>15</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E216" s="9" t="s">
         <v>845</v>
@@ -18727,7 +18706,7 @@
         <v>16</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E217" s="9" t="s">
         <v>847</v>
@@ -18768,7 +18747,7 @@
         <v>17</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E218" s="9" t="s">
         <v>848</v>
@@ -18803,7 +18782,7 @@
         <v>18</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E219" s="9" t="s">
         <v>850</v>
@@ -18841,7 +18820,7 @@
         <v>19</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E220" s="9" t="s">
         <v>853</v>
@@ -18879,7 +18858,7 @@
         <v>20</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E221" s="9" t="s">
         <v>855</v>
@@ -18914,7 +18893,7 @@
         <v>21</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E222" s="9" t="s">
         <v>857</v>
@@ -19124,7 +19103,7 @@
         <v>6</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E228" s="9" t="s">
         <v>258</v>
@@ -19159,7 +19138,7 @@
         <v>7</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="E229" s="9" t="s">
         <v>259</v>
@@ -19194,7 +19173,7 @@
         <v>8</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E230" s="9" t="s">
         <v>260</v>
@@ -19229,7 +19208,7 @@
         <v>9</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E231" s="9" t="s">
         <v>261</v>
@@ -19270,7 +19249,7 @@
         <v>10</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E232" s="9" t="s">
         <v>264</v>
@@ -19311,7 +19290,7 @@
         <v>11</v>
       </c>
       <c r="D233" s="9" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="E233" s="9" t="s">
         <v>267</v>
@@ -19346,7 +19325,7 @@
         <v>12</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="E234" s="9" t="s">
         <v>269</v>
@@ -19381,7 +19360,7 @@
         <v>13</v>
       </c>
       <c r="D235" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E235" s="9" t="s">
         <v>271</v>
@@ -19416,7 +19395,7 @@
         <v>14</v>
       </c>
       <c r="D236" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E236" s="9" t="s">
         <v>273</v>
@@ -19457,7 +19436,7 @@
         <v>15</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>2559</v>
+        <v>2546</v>
       </c>
       <c r="E237" s="9" t="s">
         <v>274</v>
@@ -19492,7 +19471,7 @@
         <v>16</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>2560</v>
+        <v>2547</v>
       </c>
       <c r="E238" s="9" t="s">
         <v>275</v>
@@ -19527,7 +19506,7 @@
         <v>17</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E239" s="9" t="s">
         <v>276</v>
@@ -19562,7 +19541,7 @@
         <v>18</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E240" s="9" t="s">
         <v>277</v>
@@ -19597,7 +19576,7 @@
         <v>19</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E241" s="9" t="s">
         <v>278</v>
@@ -19638,7 +19617,7 @@
         <v>20</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>2561</v>
+        <v>2548</v>
       </c>
       <c r="E242" s="9" t="s">
         <v>279</v>
@@ -19673,7 +19652,7 @@
         <v>21</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>2562</v>
+        <v>2549</v>
       </c>
       <c r="E243" s="9" t="s">
         <v>280</v>
@@ -19708,7 +19687,7 @@
         <v>22</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>2563</v>
+        <v>2550</v>
       </c>
       <c r="E244" s="9" t="s">
         <v>282</v>
@@ -19743,7 +19722,7 @@
         <v>23</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>2564</v>
+        <v>2551</v>
       </c>
       <c r="E245" s="9" t="s">
         <v>283</v>
@@ -19778,7 +19757,7 @@
         <v>24</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E246" s="9" t="s">
         <v>285</v>
@@ -19819,7 +19798,7 @@
         <v>25</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E247" s="9" t="s">
         <v>286</v>
@@ -19854,7 +19833,7 @@
         <v>26</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>2553</v>
+        <v>2543</v>
       </c>
       <c r="E248" s="9" t="s">
         <v>287</v>
@@ -19889,7 +19868,7 @@
         <v>27</v>
       </c>
       <c r="D249" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E249" s="9" t="s">
         <v>288</v>
@@ -19930,7 +19909,7 @@
         <v>28</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>2566</v>
+        <v>2568</v>
       </c>
       <c r="E250" s="9" t="s">
         <v>885</v>
@@ -19965,7 +19944,7 @@
         <v>29</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
       <c r="E251" s="9" t="s">
         <v>290</v>
@@ -20000,7 +19979,7 @@
         <v>30</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>2568</v>
+        <v>2573</v>
       </c>
       <c r="E252" s="9" t="s">
         <v>889</v>
@@ -20041,7 +20020,7 @@
         <v>31</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>2547</v>
+        <v>2537</v>
       </c>
       <c r="E253" s="9" t="s">
         <v>892</v>
@@ -20076,7 +20055,7 @@
         <v>32</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>2569</v>
+        <v>2574</v>
       </c>
       <c r="E254" s="9" t="s">
         <v>894</v>
@@ -20117,7 +20096,7 @@
         <v>33</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>2570</v>
+        <v>2575</v>
       </c>
       <c r="E255" s="9" t="s">
         <v>898</v>
@@ -20158,7 +20137,7 @@
         <v>34</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>2571</v>
+        <v>2576</v>
       </c>
       <c r="E256" s="9" t="s">
         <v>902</v>
@@ -20199,7 +20178,7 @@
         <v>35</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>2555</v>
+        <v>2544</v>
       </c>
       <c r="E257" s="9" t="s">
         <v>291</v>
@@ -20234,7 +20213,7 @@
         <v>36</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>2534</v>
+        <v>2529</v>
       </c>
       <c r="E258" s="9" t="s">
         <v>292</v>
@@ -20275,7 +20254,7 @@
         <v>37</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>2535</v>
+        <v>2530</v>
       </c>
       <c r="E259" s="9" t="s">
         <v>293</v>
@@ -20316,7 +20295,7 @@
         <v>38</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>2557</v>
+        <v>2545</v>
       </c>
       <c r="E260" s="9" t="s">
         <v>294</v>
@@ -20357,7 +20336,7 @@
         <v>39</v>
       </c>
       <c r="D261" s="9" t="s">
-        <v>2572</v>
+        <v>2554</v>
       </c>
       <c r="E261" s="9" t="s">
         <v>295</v>
@@ -20392,7 +20371,7 @@
         <v>40</v>
       </c>
       <c r="D262" s="9" t="s">
-        <v>2573</v>
+        <v>2555</v>
       </c>
       <c r="E262" s="9" t="s">
         <v>296</v>
@@ -20427,7 +20406,7 @@
         <v>41</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E263" s="9" t="s">
         <v>911</v>
@@ -20468,7 +20447,7 @@
         <v>42</v>
       </c>
       <c r="D264" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E264" s="9" t="s">
         <v>912</v>
@@ -20503,7 +20482,7 @@
         <v>43</v>
       </c>
       <c r="D265" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E265" s="9" t="s">
         <v>44</v>
@@ -20538,7 +20517,7 @@
         <v>44</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E266" s="9" t="s">
         <v>297</v>
@@ -20576,7 +20555,7 @@
         <v>45</v>
       </c>
       <c r="D267" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E267" s="9" t="s">
         <v>299</v>
@@ -20614,7 +20593,7 @@
         <v>46</v>
       </c>
       <c r="D268" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E268" s="9" t="s">
         <v>301</v>
@@ -20649,7 +20628,7 @@
         <v>47</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E269" s="9" t="s">
         <v>917</v>
@@ -20684,7 +20663,7 @@
         <v>48</v>
       </c>
       <c r="D270" s="9" t="s">
-        <v>2586</v>
+        <v>2565</v>
       </c>
       <c r="E270" s="9" t="s">
         <v>303</v>
@@ -20719,7 +20698,7 @@
         <v>49</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>2587</v>
+        <v>2566</v>
       </c>
       <c r="E271" s="9" t="s">
         <v>304</v>
@@ -20754,7 +20733,7 @@
         <v>50</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>2538</v>
+        <v>2578</v>
       </c>
       <c r="E272" s="9" t="s">
         <v>306</v>
@@ -20792,7 +20771,7 @@
         <v>51</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E273" s="9" t="s">
         <v>307</v>
@@ -20827,7 +20806,7 @@
         <v>52</v>
       </c>
       <c r="D274" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E274" s="9" t="s">
         <v>308</v>
@@ -21008,7 +20987,7 @@
         <v>5</v>
       </c>
       <c r="D279" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E279" s="9" t="s">
         <v>925</v>
@@ -21043,7 +21022,7 @@
         <v>6</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="E280" s="9" t="s">
         <v>927</v>
@@ -21078,7 +21057,7 @@
         <v>7</v>
       </c>
       <c r="D281" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E281" s="9" t="s">
         <v>930</v>
@@ -21113,7 +21092,7 @@
         <v>8</v>
       </c>
       <c r="D282" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E282" s="9" t="s">
         <v>932</v>
@@ -21154,7 +21133,7 @@
         <v>9</v>
       </c>
       <c r="D283" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E283" s="9" t="s">
         <v>936</v>
@@ -21195,7 +21174,7 @@
         <v>10</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>2545</v>
+        <v>2535</v>
       </c>
       <c r="E284" s="9" t="s">
         <v>940</v>
@@ -21236,7 +21215,7 @@
         <v>11</v>
       </c>
       <c r="D285" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E285" s="9" t="s">
         <v>941</v>
@@ -21271,7 +21250,7 @@
         <v>12</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E286" s="9" t="s">
         <v>943</v>
@@ -21306,7 +21285,7 @@
         <v>13</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E287" s="9" t="s">
         <v>945</v>
@@ -21347,7 +21326,7 @@
         <v>14</v>
       </c>
       <c r="D288" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E288" s="9" t="s">
         <v>947</v>
@@ -21382,7 +21361,7 @@
         <v>15</v>
       </c>
       <c r="D289" s="9" t="s">
-        <v>2553</v>
+        <v>2543</v>
       </c>
       <c r="E289" s="9" t="s">
         <v>949</v>
@@ -21417,7 +21396,7 @@
         <v>16</v>
       </c>
       <c r="D290" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E290" s="9" t="s">
         <v>952</v>
@@ -21458,7 +21437,7 @@
         <v>17</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>2566</v>
+        <v>2568</v>
       </c>
       <c r="E291" s="9" t="s">
         <v>954</v>
@@ -21493,7 +21472,7 @@
         <v>18</v>
       </c>
       <c r="D292" s="9" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
       <c r="E292" s="9" t="s">
         <v>955</v>
@@ -21528,7 +21507,7 @@
         <v>19</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>2568</v>
+        <v>2573</v>
       </c>
       <c r="E293" s="9" t="s">
         <v>957</v>
@@ -21569,7 +21548,7 @@
         <v>20</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>2569</v>
+        <v>2574</v>
       </c>
       <c r="E294" s="9" t="s">
         <v>958</v>
@@ -21610,7 +21589,7 @@
         <v>21</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>2570</v>
+        <v>2575</v>
       </c>
       <c r="E295" s="9" t="s">
         <v>959</v>
@@ -21651,7 +21630,7 @@
         <v>22</v>
       </c>
       <c r="D296" s="9" t="s">
-        <v>2571</v>
+        <v>2576</v>
       </c>
       <c r="E296" s="9" t="s">
         <v>961</v>
@@ -21692,7 +21671,7 @@
         <v>23</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E297" s="9" t="s">
         <v>962</v>
@@ -21727,7 +21706,7 @@
         <v>24</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>2549</v>
+        <v>2539</v>
       </c>
       <c r="E298" s="9" t="s">
         <v>964</v>
@@ -21768,7 +21747,7 @@
         <v>25</v>
       </c>
       <c r="D299" s="9" t="s">
-        <v>2574</v>
+        <v>2556</v>
       </c>
       <c r="E299" s="9" t="s">
         <v>966</v>
@@ -21809,7 +21788,7 @@
         <v>26</v>
       </c>
       <c r="D300" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E300" s="9" t="s">
         <v>968</v>
@@ -21847,7 +21826,7 @@
         <v>27</v>
       </c>
       <c r="D301" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E301" s="9" t="s">
         <v>970</v>
@@ -22025,7 +22004,7 @@
         <v>5</v>
       </c>
       <c r="D306" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E306" s="9" t="s">
         <v>973</v>
@@ -22060,7 +22039,7 @@
         <v>6</v>
       </c>
       <c r="D307" s="9" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="E307" s="9" t="s">
         <v>974</v>
@@ -22095,7 +22074,7 @@
         <v>7</v>
       </c>
       <c r="D308" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E308" s="9" t="s">
         <v>976</v>
@@ -22130,7 +22109,7 @@
         <v>8</v>
       </c>
       <c r="D309" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E309" s="9" t="s">
         <v>977</v>
@@ -22171,7 +22150,7 @@
         <v>9</v>
       </c>
       <c r="D310" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E310" s="9" t="s">
         <v>981</v>
@@ -22212,7 +22191,7 @@
         <v>10</v>
       </c>
       <c r="D311" s="9" t="s">
-        <v>2545</v>
+        <v>2535</v>
       </c>
       <c r="E311" s="9" t="s">
         <v>985</v>
@@ -22253,7 +22232,7 @@
         <v>11</v>
       </c>
       <c r="D312" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E312" s="9" t="s">
         <v>986</v>
@@ -22288,7 +22267,7 @@
         <v>12</v>
       </c>
       <c r="D313" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E313" s="9" t="s">
         <v>988</v>
@@ -22323,7 +22302,7 @@
         <v>13</v>
       </c>
       <c r="D314" s="9" t="s">
-        <v>2546</v>
+        <v>2536</v>
       </c>
       <c r="E314" s="9" t="s">
         <v>990</v>
@@ -22364,7 +22343,7 @@
         <v>14</v>
       </c>
       <c r="D315" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E315" s="9" t="s">
         <v>993</v>
@@ -22405,7 +22384,7 @@
         <v>15</v>
       </c>
       <c r="D316" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E316" s="9" t="s">
         <v>994</v>
@@ -22440,7 +22419,7 @@
         <v>16</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>2553</v>
+        <v>2543</v>
       </c>
       <c r="E317" s="9" t="s">
         <v>996</v>
@@ -22475,7 +22454,7 @@
         <v>17</v>
       </c>
       <c r="D318" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E318" s="9" t="s">
         <v>998</v>
@@ -22516,7 +22495,7 @@
         <v>18</v>
       </c>
       <c r="D319" s="9" t="s">
-        <v>2566</v>
+        <v>2568</v>
       </c>
       <c r="E319" s="9" t="s">
         <v>1000</v>
@@ -22551,7 +22530,7 @@
         <v>19</v>
       </c>
       <c r="D320" s="9" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
       <c r="E320" s="9" t="s">
         <v>1002</v>
@@ -22586,7 +22565,7 @@
         <v>20</v>
       </c>
       <c r="D321" s="9" t="s">
-        <v>2568</v>
+        <v>2573</v>
       </c>
       <c r="E321" s="9" t="s">
         <v>1003</v>
@@ -22627,7 +22606,7 @@
         <v>21</v>
       </c>
       <c r="D322" s="9" t="s">
-        <v>2555</v>
+        <v>2544</v>
       </c>
       <c r="E322" s="9" t="s">
         <v>1004</v>
@@ -22662,7 +22641,7 @@
         <v>22</v>
       </c>
       <c r="D323" s="9" t="s">
-        <v>2569</v>
+        <v>2574</v>
       </c>
       <c r="E323" s="9" t="s">
         <v>1006</v>
@@ -22703,7 +22682,7 @@
         <v>23</v>
       </c>
       <c r="D324" s="9" t="s">
-        <v>2570</v>
+        <v>2575</v>
       </c>
       <c r="E324" s="9" t="s">
         <v>1007</v>
@@ -22744,7 +22723,7 @@
         <v>24</v>
       </c>
       <c r="D325" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E325" s="9" t="s">
         <v>1008</v>
@@ -22779,7 +22758,7 @@
         <v>25</v>
       </c>
       <c r="D326" s="9" t="s">
-        <v>2549</v>
+        <v>2539</v>
       </c>
       <c r="E326" s="9" t="s">
         <v>1010</v>
@@ -22820,7 +22799,7 @@
         <v>26</v>
       </c>
       <c r="D327" s="9" t="s">
-        <v>2574</v>
+        <v>2556</v>
       </c>
       <c r="E327" s="9" t="s">
         <v>1012</v>
@@ -22861,7 +22840,7 @@
         <v>27</v>
       </c>
       <c r="D328" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E328" s="9" t="s">
         <v>1014</v>
@@ -22899,7 +22878,7 @@
         <v>28</v>
       </c>
       <c r="D329" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E329" s="9" t="s">
         <v>1016</v>
@@ -23077,7 +23056,7 @@
         <v>5</v>
       </c>
       <c r="D334" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E334" s="9" t="s">
         <v>1018</v>
@@ -23118,7 +23097,7 @@
         <v>6</v>
       </c>
       <c r="D335" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E335" s="9" t="s">
         <v>1021</v>
@@ -23159,7 +23138,7 @@
         <v>7</v>
       </c>
       <c r="D336" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E336" s="9" t="s">
         <v>1024</v>
@@ -23194,7 +23173,7 @@
         <v>8</v>
       </c>
       <c r="D337" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E337" s="9" t="s">
         <v>1025</v>
@@ -23235,7 +23214,7 @@
         <v>9</v>
       </c>
       <c r="D338" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E338" s="9" t="s">
         <v>1026</v>
@@ -23270,7 +23249,7 @@
         <v>10</v>
       </c>
       <c r="D339" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E339" s="9" t="s">
         <v>1028</v>
@@ -23305,7 +23284,7 @@
         <v>11</v>
       </c>
       <c r="D340" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E340" s="9" t="s">
         <v>1030</v>
@@ -23346,7 +23325,7 @@
         <v>12</v>
       </c>
       <c r="D341" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E341" s="9" t="s">
         <v>1032</v>
@@ -23387,7 +23366,7 @@
         <v>13</v>
       </c>
       <c r="D342" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E342" s="9" t="s">
         <v>1035</v>
@@ -23422,7 +23401,7 @@
         <v>14</v>
       </c>
       <c r="D343" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E343" s="9" t="s">
         <v>1037</v>
@@ -23463,7 +23442,7 @@
         <v>15</v>
       </c>
       <c r="D344" s="9" t="s">
-        <v>2566</v>
+        <v>2568</v>
       </c>
       <c r="E344" s="9" t="s">
         <v>1039</v>
@@ -23498,7 +23477,7 @@
         <v>16</v>
       </c>
       <c r="D345" s="9" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
       <c r="E345" s="9" t="s">
         <v>1041</v>
@@ -23533,7 +23512,7 @@
         <v>17</v>
       </c>
       <c r="D346" s="9" t="s">
-        <v>2568</v>
+        <v>2573</v>
       </c>
       <c r="E346" s="9" t="s">
         <v>1043</v>
@@ -23574,7 +23553,7 @@
         <v>18</v>
       </c>
       <c r="D347" s="9" t="s">
-        <v>2569</v>
+        <v>2574</v>
       </c>
       <c r="E347" s="9" t="s">
         <v>1044</v>
@@ -23615,7 +23594,7 @@
         <v>19</v>
       </c>
       <c r="D348" s="9" t="s">
-        <v>2570</v>
+        <v>2575</v>
       </c>
       <c r="E348" s="9" t="s">
         <v>1045</v>
@@ -23656,7 +23635,7 @@
         <v>20</v>
       </c>
       <c r="D349" s="9" t="s">
-        <v>2571</v>
+        <v>2576</v>
       </c>
       <c r="E349" s="9" t="s">
         <v>1046</v>
@@ -23697,7 +23676,7 @@
         <v>21</v>
       </c>
       <c r="D350" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E350" s="9" t="s">
         <v>1047</v>
@@ -23738,7 +23717,7 @@
         <v>22</v>
       </c>
       <c r="D351" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E351" s="9" t="s">
         <v>1048</v>
@@ -23773,7 +23752,7 @@
         <v>23</v>
       </c>
       <c r="D352" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E352" s="9" t="s">
         <v>1050</v>
@@ -23811,7 +23790,7 @@
         <v>24</v>
       </c>
       <c r="D353" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E353" s="9" t="s">
         <v>1053</v>
@@ -23989,7 +23968,7 @@
         <v>5</v>
       </c>
       <c r="D358" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E358" s="9" t="s">
         <v>1057</v>
@@ -24024,7 +24003,7 @@
         <v>6</v>
       </c>
       <c r="D359" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E359" s="9" t="s">
         <v>1058</v>
@@ -24059,7 +24038,7 @@
         <v>7</v>
       </c>
       <c r="D360" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E360" s="9" t="s">
         <v>1059</v>
@@ -24100,7 +24079,7 @@
         <v>8</v>
       </c>
       <c r="D361" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E361" s="9" t="s">
         <v>1062</v>
@@ -24141,7 +24120,7 @@
         <v>9</v>
       </c>
       <c r="D362" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E362" s="9" t="s">
         <v>1065</v>
@@ -24176,7 +24155,7 @@
         <v>10</v>
       </c>
       <c r="D363" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E363" s="9" t="s">
         <v>1067</v>
@@ -24217,7 +24196,7 @@
         <v>11</v>
       </c>
       <c r="D364" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E364" s="9" t="s">
         <v>1069</v>
@@ -24252,7 +24231,7 @@
         <v>12</v>
       </c>
       <c r="D365" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E365" s="9" t="s">
         <v>1071</v>
@@ -24287,7 +24266,7 @@
         <v>13</v>
       </c>
       <c r="D366" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E366" s="9" t="s">
         <v>1073</v>
@@ -24328,7 +24307,7 @@
         <v>14</v>
       </c>
       <c r="D367" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E367" s="9" t="s">
         <v>1075</v>
@@ -24369,7 +24348,7 @@
         <v>15</v>
       </c>
       <c r="D368" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E368" s="9" t="s">
         <v>1077</v>
@@ -24404,7 +24383,7 @@
         <v>16</v>
       </c>
       <c r="D369" s="9" t="s">
-        <v>2547</v>
+        <v>2537</v>
       </c>
       <c r="E369" s="9" t="s">
         <v>1079</v>
@@ -24439,7 +24418,7 @@
         <v>17</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E370" s="9" t="s">
         <v>1081</v>
@@ -24474,7 +24453,7 @@
         <v>18</v>
       </c>
       <c r="D371" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E371" s="9" t="s">
         <v>44</v>
@@ -24509,7 +24488,7 @@
         <v>19</v>
       </c>
       <c r="D372" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E372" s="9" t="s">
         <v>1083</v>
@@ -24547,7 +24526,7 @@
         <v>20</v>
       </c>
       <c r="D373" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E373" s="9" t="s">
         <v>1085</v>
@@ -24757,7 +24736,7 @@
         <v>6</v>
       </c>
       <c r="D379" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E379" s="9" t="s">
         <v>312</v>
@@ -24792,7 +24771,7 @@
         <v>7</v>
       </c>
       <c r="D380" s="9" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="E380" s="9" t="s">
         <v>313</v>
@@ -24827,7 +24806,7 @@
         <v>8</v>
       </c>
       <c r="D381" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E381" s="9" t="s">
         <v>314</v>
@@ -24862,7 +24841,7 @@
         <v>9</v>
       </c>
       <c r="D382" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E382" s="9" t="s">
         <v>316</v>
@@ -24897,7 +24876,7 @@
         <v>10</v>
       </c>
       <c r="D383" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E383" s="9" t="s">
         <v>317</v>
@@ -24932,7 +24911,7 @@
         <v>11</v>
       </c>
       <c r="D384" s="9" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="E384" s="9" t="s">
         <v>318</v>
@@ -24967,7 +24946,7 @@
         <v>12</v>
       </c>
       <c r="D385" s="9" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="E385" s="9" t="s">
         <v>321</v>
@@ -25002,7 +24981,7 @@
         <v>13</v>
       </c>
       <c r="D386" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E386" s="9" t="s">
         <v>324</v>
@@ -25037,7 +25016,7 @@
         <v>14</v>
       </c>
       <c r="D387" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E387" s="9" t="s">
         <v>325</v>
@@ -25078,7 +25057,7 @@
         <v>15</v>
       </c>
       <c r="D388" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E388" s="9" t="s">
         <v>326</v>
@@ -25113,7 +25092,7 @@
         <v>16</v>
       </c>
       <c r="D389" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E389" s="9" t="s">
         <v>327</v>
@@ -25148,7 +25127,7 @@
         <v>17</v>
       </c>
       <c r="D390" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E390" s="9" t="s">
         <v>328</v>
@@ -25189,7 +25168,7 @@
         <v>18</v>
       </c>
       <c r="D391" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E391" s="9" t="s">
         <v>330</v>
@@ -25230,7 +25209,7 @@
         <v>19</v>
       </c>
       <c r="D392" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E392" s="9" t="s">
         <v>331</v>
@@ -25265,7 +25244,7 @@
         <v>20</v>
       </c>
       <c r="D393" s="9" t="s">
-        <v>2553</v>
+        <v>2543</v>
       </c>
       <c r="E393" s="9" t="s">
         <v>332</v>
@@ -25300,7 +25279,7 @@
         <v>21</v>
       </c>
       <c r="D394" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E394" s="9" t="s">
         <v>333</v>
@@ -25341,7 +25320,7 @@
         <v>22</v>
       </c>
       <c r="D395" s="9" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
       <c r="E395" s="9" t="s">
         <v>334</v>
@@ -25376,7 +25355,7 @@
         <v>23</v>
       </c>
       <c r="D396" s="9" t="s">
-        <v>2555</v>
+        <v>2544</v>
       </c>
       <c r="E396" s="9" t="s">
         <v>335</v>
@@ -25411,7 +25390,7 @@
         <v>24</v>
       </c>
       <c r="D397" s="9" t="s">
-        <v>2534</v>
+        <v>2529</v>
       </c>
       <c r="E397" s="9" t="s">
         <v>1100</v>
@@ -25452,7 +25431,7 @@
         <v>25</v>
       </c>
       <c r="D398" s="9" t="s">
-        <v>2535</v>
+        <v>2530</v>
       </c>
       <c r="E398" s="9" t="s">
         <v>337</v>
@@ -25493,7 +25472,7 @@
         <v>26</v>
       </c>
       <c r="D399" s="9" t="s">
-        <v>2557</v>
+        <v>2545</v>
       </c>
       <c r="E399" s="9" t="s">
         <v>338</v>
@@ -25534,7 +25513,7 @@
         <v>27</v>
       </c>
       <c r="D400" s="9" t="s">
-        <v>2575</v>
+        <v>2557</v>
       </c>
       <c r="E400" s="9" t="s">
         <v>339</v>
@@ -25569,7 +25548,7 @@
         <v>28</v>
       </c>
       <c r="D401" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E401" s="9" t="s">
         <v>1102</v>
@@ -25610,7 +25589,7 @@
         <v>29</v>
       </c>
       <c r="D402" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E402" s="9" t="s">
         <v>1104</v>
@@ -25645,7 +25624,7 @@
         <v>30</v>
       </c>
       <c r="D403" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E403" s="9" t="s">
         <v>44</v>
@@ -25680,7 +25659,7 @@
         <v>31</v>
       </c>
       <c r="D404" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E404" s="9" t="s">
         <v>341</v>
@@ -25718,7 +25697,7 @@
         <v>32</v>
       </c>
       <c r="D405" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E405" s="9" t="s">
         <v>342</v>
@@ -25756,7 +25735,7 @@
         <v>33</v>
       </c>
       <c r="D406" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E406" s="9" t="s">
         <v>343</v>
@@ -25791,7 +25770,7 @@
         <v>34</v>
       </c>
       <c r="D407" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E407" s="9" t="s">
         <v>1111</v>
@@ -25826,7 +25805,7 @@
         <v>35</v>
       </c>
       <c r="D408" s="9" t="s">
-        <v>2586</v>
+        <v>2565</v>
       </c>
       <c r="E408" s="9" t="s">
         <v>344</v>
@@ -25861,7 +25840,7 @@
         <v>36</v>
       </c>
       <c r="D409" s="9" t="s">
-        <v>2587</v>
+        <v>2566</v>
       </c>
       <c r="E409" s="9" t="s">
         <v>345</v>
@@ -25896,7 +25875,7 @@
         <v>37</v>
       </c>
       <c r="D410" s="9" t="s">
-        <v>2538</v>
+        <v>2578</v>
       </c>
       <c r="E410" s="9" t="s">
         <v>347</v>
@@ -25934,7 +25913,7 @@
         <v>38</v>
       </c>
       <c r="D411" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E411" s="9" t="s">
         <v>348</v>
@@ -25969,7 +25948,7 @@
         <v>39</v>
       </c>
       <c r="D412" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E412" s="9" t="s">
         <v>350</v>
@@ -26007,7 +25986,7 @@
         <v>40</v>
       </c>
       <c r="D413" s="9" t="s">
-        <v>2558</v>
+        <v>2581</v>
       </c>
       <c r="E413" s="9" t="s">
         <v>353</v>
@@ -26220,7 +26199,7 @@
         <v>6</v>
       </c>
       <c r="D419" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E419" s="9" t="s">
         <v>355</v>
@@ -26255,7 +26234,7 @@
         <v>7</v>
       </c>
       <c r="D420" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E420" s="9" t="s">
         <v>356</v>
@@ -26296,7 +26275,7 @@
         <v>8</v>
       </c>
       <c r="D421" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E421" s="9" t="s">
         <v>358</v>
@@ -26337,7 +26316,7 @@
         <v>9</v>
       </c>
       <c r="D422" s="9" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="E422" s="9" t="s">
         <v>360</v>
@@ -26372,7 +26351,7 @@
         <v>10</v>
       </c>
       <c r="D423" s="9" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="E423" s="9" t="s">
         <v>363</v>
@@ -26407,7 +26386,7 @@
         <v>11</v>
       </c>
       <c r="D424" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E424" s="9" t="s">
         <v>365</v>
@@ -26442,7 +26421,7 @@
         <v>12</v>
       </c>
       <c r="D425" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E425" s="9" t="s">
         <v>366</v>
@@ -26483,7 +26462,7 @@
         <v>13</v>
       </c>
       <c r="D426" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E426" s="9" t="s">
         <v>367</v>
@@ -26518,7 +26497,7 @@
         <v>14</v>
       </c>
       <c r="D427" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E427" s="9" t="s">
         <v>368</v>
@@ -26553,7 +26532,7 @@
         <v>15</v>
       </c>
       <c r="D428" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E428" s="9" t="s">
         <v>369</v>
@@ -26594,7 +26573,7 @@
         <v>16</v>
       </c>
       <c r="D429" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E429" s="9" t="s">
         <v>371</v>
@@ -26635,7 +26614,7 @@
         <v>17</v>
       </c>
       <c r="D430" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E430" s="9" t="s">
         <v>373</v>
@@ -26670,7 +26649,7 @@
         <v>18</v>
       </c>
       <c r="D431" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E431" s="9" t="s">
         <v>374</v>
@@ -26711,7 +26690,7 @@
         <v>19</v>
       </c>
       <c r="D432" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E432" s="9" t="s">
         <v>44</v>
@@ -26746,7 +26725,7 @@
         <v>20</v>
       </c>
       <c r="D433" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E433" s="9" t="s">
         <v>1129</v>
@@ -26781,7 +26760,7 @@
         <v>21</v>
       </c>
       <c r="D434" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E434" s="9" t="s">
         <v>375</v>
@@ -26818,9 +26797,6 @@
       <c r="C435" s="13">
         <v>22</v>
       </c>
-      <c r="D435" s="9" t="s">
-        <v>2576</v>
-      </c>
       <c r="E435" s="9" t="s">
         <v>1131</v>
       </c>
@@ -26856,9 +26832,6 @@
       <c r="C436" s="13">
         <v>23</v>
       </c>
-      <c r="D436" s="9" t="s">
-        <v>2577</v>
-      </c>
       <c r="E436" s="9" t="s">
         <v>1134</v>
       </c>
@@ -27038,7 +27011,7 @@
         <v>5</v>
       </c>
       <c r="D441" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E441" s="9" t="s">
         <v>385</v>
@@ -27073,7 +27046,7 @@
         <v>6</v>
       </c>
       <c r="D442" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E442" s="9" t="s">
         <v>386</v>
@@ -27114,7 +27087,7 @@
         <v>7</v>
       </c>
       <c r="D443" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E443" s="9" t="s">
         <v>388</v>
@@ -27155,7 +27128,7 @@
         <v>8</v>
       </c>
       <c r="D444" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E444" s="9" t="s">
         <v>390</v>
@@ -27190,7 +27163,7 @@
         <v>9</v>
       </c>
       <c r="D445" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E445" s="9" t="s">
         <v>392</v>
@@ -27231,7 +27204,7 @@
         <v>10</v>
       </c>
       <c r="D446" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E446" s="9" t="s">
         <v>393</v>
@@ -27266,7 +27239,7 @@
         <v>11</v>
       </c>
       <c r="D447" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E447" s="9" t="s">
         <v>394</v>
@@ -27301,7 +27274,7 @@
         <v>12</v>
       </c>
       <c r="D448" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E448" s="9" t="s">
         <v>395</v>
@@ -27342,7 +27315,7 @@
         <v>13</v>
       </c>
       <c r="D449" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E449" s="9" t="s">
         <v>397</v>
@@ -27380,7 +27353,7 @@
         <v>14</v>
       </c>
       <c r="D450" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E450" s="9" t="s">
         <v>398</v>
@@ -27558,7 +27531,7 @@
         <v>5</v>
       </c>
       <c r="D455" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E455" s="9" t="s">
         <v>1147</v>
@@ -27593,7 +27566,7 @@
         <v>6</v>
       </c>
       <c r="D456" s="9" t="s">
-        <v>2550</v>
+        <v>2540</v>
       </c>
       <c r="E456" s="9" t="s">
         <v>1148</v>
@@ -27628,7 +27601,7 @@
         <v>7</v>
       </c>
       <c r="D457" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E457" s="9" t="s">
         <v>1149</v>
@@ -27663,7 +27636,7 @@
         <v>8</v>
       </c>
       <c r="D458" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E458" s="9" t="s">
         <v>1151</v>
@@ -27704,7 +27677,7 @@
         <v>9</v>
       </c>
       <c r="D459" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E459" s="9" t="s">
         <v>1155</v>
@@ -27745,7 +27718,7 @@
         <v>10</v>
       </c>
       <c r="D460" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E460" s="9" t="s">
         <v>1159</v>
@@ -27780,7 +27753,7 @@
         <v>11</v>
       </c>
       <c r="D461" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E461" s="9" t="s">
         <v>1161</v>
@@ -27821,7 +27794,7 @@
         <v>12</v>
       </c>
       <c r="D462" s="9" t="s">
-        <v>2546</v>
+        <v>2536</v>
       </c>
       <c r="E462" s="9" t="s">
         <v>1164</v>
@@ -27862,7 +27835,7 @@
         <v>13</v>
       </c>
       <c r="D463" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E463" s="9" t="s">
         <v>1168</v>
@@ -27903,7 +27876,7 @@
         <v>14</v>
       </c>
       <c r="D464" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E464" s="9" t="s">
         <v>1170</v>
@@ -27970,7 +27943,7 @@
         <v>16</v>
       </c>
       <c r="D466" s="9" t="s">
-        <v>2565</v>
+        <v>2552</v>
       </c>
       <c r="E466" s="9" t="s">
         <v>1173</v>
@@ -28011,7 +27984,7 @@
         <v>17</v>
       </c>
       <c r="D467" s="9" t="s">
-        <v>2566</v>
+        <v>2568</v>
       </c>
       <c r="E467" s="9" t="s">
         <v>1175</v>
@@ -28046,7 +28019,7 @@
         <v>18</v>
       </c>
       <c r="D468" s="9" t="s">
-        <v>2567</v>
+        <v>2553</v>
       </c>
       <c r="E468" s="9" t="s">
         <v>1177</v>
@@ -28081,7 +28054,7 @@
         <v>19</v>
       </c>
       <c r="D469" s="9" t="s">
-        <v>2555</v>
+        <v>2544</v>
       </c>
       <c r="E469" s="9" t="s">
         <v>1179</v>
@@ -28116,7 +28089,7 @@
         <v>20</v>
       </c>
       <c r="D470" s="9" t="s">
-        <v>2569</v>
+        <v>2574</v>
       </c>
       <c r="E470" s="9" t="s">
         <v>1181</v>
@@ -28157,7 +28130,7 @@
         <v>21</v>
       </c>
       <c r="D471" s="9" t="s">
-        <v>2570</v>
+        <v>2575</v>
       </c>
       <c r="E471" s="9" t="s">
         <v>1182</v>
@@ -28198,7 +28171,7 @@
         <v>22</v>
       </c>
       <c r="D472" s="9" t="s">
-        <v>2548</v>
+        <v>2538</v>
       </c>
       <c r="E472" s="9" t="s">
         <v>1183</v>
@@ -28233,7 +28206,7 @@
         <v>23</v>
       </c>
       <c r="D473" s="9" t="s">
-        <v>2574</v>
+        <v>2556</v>
       </c>
       <c r="E473" s="9" t="s">
         <v>1184</v>
@@ -28274,7 +28247,7 @@
         <v>24</v>
       </c>
       <c r="D474" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E474" s="9" t="s">
         <v>1186</v>
@@ -28312,7 +28285,7 @@
         <v>25</v>
       </c>
       <c r="D475" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E475" s="9" t="s">
         <v>1187</v>
@@ -28347,7 +28320,7 @@
         <v>26</v>
       </c>
       <c r="D476" s="9" t="s">
-        <v>2578</v>
+        <v>2582</v>
       </c>
       <c r="E476" s="9" t="s">
         <v>1188</v>
@@ -28522,7 +28495,7 @@
         <v>5</v>
       </c>
       <c r="D481" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E481" s="9" t="s">
         <v>450</v>
@@ -28557,7 +28530,7 @@
         <v>6</v>
       </c>
       <c r="D482" s="9" t="s">
-        <v>2542</v>
+        <v>2532</v>
       </c>
       <c r="E482" s="9" t="s">
         <v>451</v>
@@ -28592,7 +28565,7 @@
         <v>7</v>
       </c>
       <c r="D483" s="9" t="s">
-        <v>2525</v>
+        <v>2520</v>
       </c>
       <c r="E483" s="9" t="s">
         <v>452</v>
@@ -28633,7 +28606,7 @@
         <v>8</v>
       </c>
       <c r="D484" s="9" t="s">
-        <v>2526</v>
+        <v>2521</v>
       </c>
       <c r="E484" s="9" t="s">
         <v>455</v>
@@ -28674,7 +28647,7 @@
         <v>9</v>
       </c>
       <c r="D485" s="9" t="s">
-        <v>2543</v>
+        <v>2533</v>
       </c>
       <c r="E485" s="9" t="s">
         <v>458</v>
@@ -28709,7 +28682,7 @@
         <v>10</v>
       </c>
       <c r="D486" s="9" t="s">
-        <v>2544</v>
+        <v>2534</v>
       </c>
       <c r="E486" s="9" t="s">
         <v>460</v>
@@ -28744,7 +28717,7 @@
         <v>11</v>
       </c>
       <c r="D487" s="9" t="s">
-        <v>2551</v>
+        <v>2541</v>
       </c>
       <c r="E487" s="9" t="s">
         <v>463</v>
@@ -28785,7 +28758,7 @@
         <v>12</v>
       </c>
       <c r="D488" s="9" t="s">
-        <v>2527</v>
+        <v>2522</v>
       </c>
       <c r="E488" s="9" t="s">
         <v>465</v>
@@ -28820,7 +28793,7 @@
         <v>13</v>
       </c>
       <c r="D489" s="9" t="s">
-        <v>2528</v>
+        <v>2523</v>
       </c>
       <c r="E489" s="9" t="s">
         <v>467</v>
@@ -28861,7 +28834,7 @@
         <v>14</v>
       </c>
       <c r="D490" s="9" t="s">
-        <v>2529</v>
+        <v>2524</v>
       </c>
       <c r="E490" s="9" t="s">
         <v>469</v>
@@ -28896,7 +28869,7 @@
         <v>15</v>
       </c>
       <c r="D491" s="9" t="s">
-        <v>2530</v>
+        <v>2525</v>
       </c>
       <c r="E491" s="9" t="s">
         <v>470</v>
@@ -28931,7 +28904,7 @@
         <v>16</v>
       </c>
       <c r="D492" s="9" t="s">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E492" s="9" t="s">
         <v>472</v>
@@ -28972,7 +28945,7 @@
         <v>17</v>
       </c>
       <c r="D493" s="9" t="s">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="E493" s="9" t="s">
         <v>473</v>
@@ -29013,7 +28986,7 @@
         <v>18</v>
       </c>
       <c r="D494" s="9" t="s">
-        <v>2533</v>
+        <v>2528</v>
       </c>
       <c r="E494" s="9" t="s">
         <v>474</v>
@@ -29048,7 +29021,7 @@
         <v>19</v>
       </c>
       <c r="D495" s="9" t="s">
-        <v>2547</v>
+        <v>2537</v>
       </c>
       <c r="E495" s="9" t="s">
         <v>475</v>
@@ -29083,7 +29056,7 @@
         <v>20</v>
       </c>
       <c r="D496" s="9" t="s">
-        <v>2556</v>
+        <v>2572</v>
       </c>
       <c r="E496" s="9" t="s">
         <v>1196</v>
@@ -29124,7 +29097,7 @@
         <v>21</v>
       </c>
       <c r="D497" s="9" t="s">
-        <v>2534</v>
+        <v>2529</v>
       </c>
       <c r="E497" s="9" t="s">
         <v>478</v>
@@ -29165,7 +29138,7 @@
         <v>22</v>
       </c>
       <c r="D498" s="9" t="s">
-        <v>2557</v>
+        <v>2545</v>
       </c>
       <c r="E498" s="9" t="s">
         <v>479</v>
@@ -29200,7 +29173,7 @@
         <v>23</v>
       </c>
       <c r="D499" s="9" t="s">
-        <v>2536</v>
+        <v>2569</v>
       </c>
       <c r="E499" s="9" t="s">
         <v>1199</v>
@@ -29241,7 +29214,7 @@
         <v>24</v>
       </c>
       <c r="D500" s="9" t="s">
-        <v>2537</v>
+        <v>2570</v>
       </c>
       <c r="E500" s="9" t="s">
         <v>1200</v>
@@ -29276,7 +29249,7 @@
         <v>25</v>
       </c>
       <c r="D501" s="9" t="s">
-        <v>2588</v>
+        <v>2567</v>
       </c>
       <c r="E501" s="9" t="s">
         <v>44</v>
@@ -29311,7 +29284,7 @@
         <v>26</v>
       </c>
       <c r="D502" s="9" t="s">
-        <v>2582</v>
+        <v>2561</v>
       </c>
       <c r="E502" s="9" t="s">
         <v>480</v>
@@ -29349,7 +29322,7 @@
         <v>27</v>
       </c>
       <c r="D503" s="9" t="s">
-        <v>2581</v>
+        <v>2560</v>
       </c>
       <c r="E503" s="9" t="s">
         <v>1204</v>
@@ -29387,7 +29360,7 @@
         <v>28</v>
       </c>
       <c r="D504" s="9" t="s">
-        <v>2583</v>
+        <v>2562</v>
       </c>
       <c r="E504" s="9" t="s">
         <v>481</v>
@@ -29422,7 +29395,7 @@
         <v>29</v>
       </c>
       <c r="D505" s="9" t="s">
-        <v>2585</v>
+        <v>2564</v>
       </c>
       <c r="E505" s="9" t="s">
         <v>1209</v>
@@ -29457,7 +29430,7 @@
         <v>30</v>
       </c>
       <c r="D506" s="9" t="s">
-        <v>2586</v>
+        <v>2565</v>
       </c>
       <c r="E506" s="9" t="s">
         <v>482</v>
@@ -29492,7 +29465,7 @@
         <v>31</v>
       </c>
       <c r="D507" s="9" t="s">
-        <v>2587</v>
+        <v>2566</v>
       </c>
       <c r="E507" s="9" t="s">
         <v>483</v>
@@ -29527,7 +29500,7 @@
         <v>32</v>
       </c>
       <c r="D508" s="9" t="s">
-        <v>2538</v>
+        <v>2578</v>
       </c>
       <c r="E508" s="9" t="s">
         <v>484</v>
@@ -29565,7 +29538,7 @@
         <v>33</v>
       </c>
       <c r="D509" s="9" t="s">
-        <v>2539</v>
+        <v>2579</v>
       </c>
       <c r="E509" s="9" t="s">
         <v>485</v>
@@ -29600,7 +29573,7 @@
         <v>34</v>
       </c>
       <c r="D510" s="9" t="s">
-        <v>2540</v>
+        <v>2580</v>
       </c>
       <c r="E510" s="9" t="s">
         <v>487</v>
@@ -30171,7 +30144,7 @@
         <v>10</v>
       </c>
       <c r="D527" s="9" t="s">
-        <v>2579</v>
+        <v>2558</v>
       </c>
       <c r="E527" s="9" t="s">
         <v>47</v>
@@ -30594,7 +30567,7 @@
         <v>4</v>
       </c>
       <c r="D539" s="9" t="s">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="E539" s="9" t="s">
         <v>442</v>

</xml_diff>